<commit_message>
#1 remove empty DCC file
</commit_message>
<xml_diff>
--- a/inst/extdata/WTA_NGS_Example/annotation/kidney_AOI_Annotations_all_vignette.xlsx
+++ b/inst/extdata/WTA_NGS_Example/annotation/kidney_AOI_Annotations_all_vignette.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jreeves\Documents\DA Vignettes\GeoMxWorkflows\annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jreeves\Documents\R\Github\GeoMxWorkflows\inst\extdata\WTA_NGS_Example\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8709C311-95C5-48F7-A07A-67A21AC42FC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B766D64D-E37C-4EC7-BFA6-4DFB0923A2FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="3330" windowWidth="25425" windowHeight="11760" xr2:uid="{776D697D-50BF-449B-A436-D86E0F27716D}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20430" windowHeight="11385" xr2:uid="{776D697D-50BF-449B-A436-D86E0F27716D}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="271">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -415,9 +415,6 @@
   </si>
   <si>
     <t>DSP-1001250007864-D-C09</t>
-  </si>
-  <si>
-    <t>DSP-1001250007864-D-C10</t>
   </si>
   <si>
     <t>DSP-1001250007864-D-C11</t>
@@ -1221,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D2ABA0-3808-4F97-A08C-4FABCCAEED45}">
-  <dimension ref="A1:K241"/>
+  <dimension ref="A1:K240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1265,7 +1262,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2949,10 +2946,10 @@
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H50" s="1">
         <v>23053.27</v>
@@ -2984,10 +2981,10 @@
         <v>1</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H51" s="1">
         <v>137927.28</v>
@@ -3019,10 +3016,10 @@
         <v>2</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H52" s="1">
         <v>17553.53</v>
@@ -3054,10 +3051,10 @@
         <v>2</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H53" s="1">
         <v>123467.45</v>
@@ -3089,10 +3086,10 @@
         <v>3</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H54" s="1">
         <v>22011.87</v>
@@ -3124,10 +3121,10 @@
         <v>3</v>
       </c>
       <c r="F55" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H55" s="1">
         <v>209925.63</v>
@@ -3159,10 +3156,10 @@
         <v>4</v>
       </c>
       <c r="F56" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H56" s="1">
         <v>17157.169999999998</v>
@@ -3194,10 +3191,10 @@
         <v>4</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H57" s="1">
         <v>145616.81</v>
@@ -3229,10 +3226,10 @@
         <v>5</v>
       </c>
       <c r="F58" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H58" s="1">
         <v>10254.219999999999</v>
@@ -3264,10 +3261,10 @@
         <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H59" s="1">
         <v>105417.67</v>
@@ -3299,10 +3296,10 @@
         <v>6</v>
       </c>
       <c r="F60" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H60" s="1">
         <v>34076.47</v>
@@ -3334,10 +3331,10 @@
         <v>6</v>
       </c>
       <c r="F61" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H61" s="1">
         <v>137743.29999999999</v>
@@ -3808,10 +3805,10 @@
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H75" s="1">
         <v>20265.55</v>
@@ -3843,10 +3840,10 @@
         <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H76" s="1">
         <v>91483.62</v>
@@ -3878,10 +3875,10 @@
         <v>2</v>
       </c>
       <c r="F77" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H77" s="1">
         <v>12966.08</v>
@@ -3913,10 +3910,10 @@
         <v>2</v>
       </c>
       <c r="F78" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G78" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H78" s="1">
         <v>133866.42000000001</v>
@@ -3948,10 +3945,10 @@
         <v>3</v>
       </c>
       <c r="F79" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H79" s="1">
         <v>23336.81</v>
@@ -3983,10 +3980,10 @@
         <v>3</v>
       </c>
       <c r="F80" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H80" s="1">
         <v>174741.6</v>
@@ -4018,10 +4015,10 @@
         <v>4</v>
       </c>
       <c r="F81" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H81" s="1">
         <v>15875.8</v>
@@ -4053,10 +4050,10 @@
         <v>4</v>
       </c>
       <c r="F82" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H82" s="1">
         <v>122888.57</v>
@@ -4088,10 +4085,10 @@
         <v>5</v>
       </c>
       <c r="F83" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H83" s="1">
         <v>23311.32</v>
@@ -4123,10 +4120,10 @@
         <v>5</v>
       </c>
       <c r="F84" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H84" s="1">
         <v>89287.05</v>
@@ -4158,10 +4155,10 @@
         <v>6</v>
       </c>
       <c r="F85" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="H85" s="1">
         <v>9671.7900000000009</v>
@@ -4193,10 +4190,10 @@
         <v>6</v>
       </c>
       <c r="F86" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="H86" s="1">
         <v>77969.649999999994</v>
@@ -4925,7 +4922,7 @@
         <v>81</v>
       </c>
       <c r="E107" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>15</v>
@@ -4934,7 +4931,7 @@
         <v>16</v>
       </c>
       <c r="H107" s="1">
-        <v>27705.91</v>
+        <v>35146.269999999997</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>17</v>
@@ -4943,7 +4940,7 @@
         <v>81</v>
       </c>
       <c r="K107" s="1">
-        <v>108</v>
+        <v>158</v>
       </c>
     </row>
     <row r="108" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -4960,7 +4957,7 @@
         <v>81</v>
       </c>
       <c r="E108" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>15</v>
@@ -4969,7 +4966,7 @@
         <v>16</v>
       </c>
       <c r="H108" s="1">
-        <v>35146.269999999997</v>
+        <v>30810.9</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>17</v>
@@ -4978,7 +4975,7 @@
         <v>81</v>
       </c>
       <c r="K108" s="1">
-        <v>158</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -4995,7 +4992,7 @@
         <v>81</v>
       </c>
       <c r="E109" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>15</v>
@@ -5004,7 +5001,7 @@
         <v>16</v>
       </c>
       <c r="H109" s="1">
-        <v>30810.9</v>
+        <v>27445.119999999999</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>17</v>
@@ -5013,7 +5010,7 @@
         <v>81</v>
       </c>
       <c r="K109" s="1">
-        <v>178</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5030,7 +5027,7 @@
         <v>81</v>
       </c>
       <c r="E110" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>15</v>
@@ -5039,7 +5036,7 @@
         <v>16</v>
       </c>
       <c r="H110" s="1">
-        <v>27445.119999999999</v>
+        <v>49933.55</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>17</v>
@@ -5048,7 +5045,7 @@
         <v>81</v>
       </c>
       <c r="K110" s="1">
-        <v>130</v>
+        <v>255</v>
       </c>
     </row>
     <row r="111" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5065,7 +5062,7 @@
         <v>81</v>
       </c>
       <c r="E111" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>15</v>
@@ -5074,7 +5071,7 @@
         <v>16</v>
       </c>
       <c r="H111" s="1">
-        <v>49933.55</v>
+        <v>41998.39</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>17</v>
@@ -5083,7 +5080,7 @@
         <v>81</v>
       </c>
       <c r="K111" s="1">
-        <v>255</v>
+        <v>223</v>
       </c>
     </row>
     <row r="112" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5100,7 +5097,7 @@
         <v>81</v>
       </c>
       <c r="E112" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>15</v>
@@ -5109,7 +5106,7 @@
         <v>16</v>
       </c>
       <c r="H112" s="1">
-        <v>41998.39</v>
+        <v>31837.78</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>17</v>
@@ -5118,7 +5115,7 @@
         <v>81</v>
       </c>
       <c r="K112" s="1">
-        <v>223</v>
+        <v>164</v>
       </c>
     </row>
     <row r="113" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5135,7 +5132,7 @@
         <v>81</v>
       </c>
       <c r="E113" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>15</v>
@@ -5144,7 +5141,7 @@
         <v>16</v>
       </c>
       <c r="H113" s="1">
-        <v>31837.78</v>
+        <v>20978.54</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>17</v>
@@ -5153,7 +5150,7 @@
         <v>81</v>
       </c>
       <c r="K113" s="1">
-        <v>164</v>
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5170,7 +5167,7 @@
         <v>81</v>
       </c>
       <c r="E114" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>15</v>
@@ -5179,7 +5176,7 @@
         <v>16</v>
       </c>
       <c r="H114" s="1">
-        <v>20978.54</v>
+        <v>25290.51</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>17</v>
@@ -5188,7 +5185,7 @@
         <v>81</v>
       </c>
       <c r="K114" s="1">
-        <v>100</v>
+        <v>127</v>
       </c>
     </row>
     <row r="115" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5205,7 +5202,7 @@
         <v>81</v>
       </c>
       <c r="E115" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>15</v>
@@ -5214,7 +5211,7 @@
         <v>16</v>
       </c>
       <c r="H115" s="1">
-        <v>25290.51</v>
+        <v>25689.599999999999</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>17</v>
@@ -5223,7 +5220,7 @@
         <v>81</v>
       </c>
       <c r="K115" s="1">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="116" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5240,7 +5237,7 @@
         <v>81</v>
       </c>
       <c r="E116" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>15</v>
@@ -5249,7 +5246,7 @@
         <v>16</v>
       </c>
       <c r="H116" s="1">
-        <v>25689.599999999999</v>
+        <v>34535.599999999999</v>
       </c>
       <c r="I116" s="1" t="s">
         <v>17</v>
@@ -5258,7 +5255,7 @@
         <v>81</v>
       </c>
       <c r="K116" s="1">
-        <v>132</v>
+        <v>181</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5275,7 +5272,7 @@
         <v>81</v>
       </c>
       <c r="E117" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>15</v>
@@ -5284,7 +5281,7 @@
         <v>16</v>
       </c>
       <c r="H117" s="1">
-        <v>34535.599999999999</v>
+        <v>24650.3</v>
       </c>
       <c r="I117" s="1" t="s">
         <v>17</v>
@@ -5293,7 +5290,7 @@
         <v>81</v>
       </c>
       <c r="K117" s="1">
-        <v>181</v>
+        <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5310,7 +5307,7 @@
         <v>81</v>
       </c>
       <c r="E118" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>15</v>
@@ -5319,7 +5316,7 @@
         <v>16</v>
       </c>
       <c r="H118" s="1">
-        <v>24650.3</v>
+        <v>18153.22</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>17</v>
@@ -5328,7 +5325,7 @@
         <v>81</v>
       </c>
       <c r="K118" s="1">
-        <v>128</v>
+        <v>83</v>
       </c>
     </row>
     <row r="119" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5345,7 +5342,7 @@
         <v>81</v>
       </c>
       <c r="E119" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>15</v>
@@ -5354,7 +5351,7 @@
         <v>16</v>
       </c>
       <c r="H119" s="1">
-        <v>18153.22</v>
+        <v>20003.47</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>17</v>
@@ -5363,7 +5360,7 @@
         <v>81</v>
       </c>
       <c r="K119" s="1">
-        <v>83</v>
+        <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5380,7 +5377,7 @@
         <v>81</v>
       </c>
       <c r="E120" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>15</v>
@@ -5389,7 +5386,7 @@
         <v>16</v>
       </c>
       <c r="H120" s="1">
-        <v>20003.47</v>
+        <v>30229.279999999999</v>
       </c>
       <c r="I120" s="1" t="s">
         <v>17</v>
@@ -5398,7 +5395,7 @@
         <v>81</v>
       </c>
       <c r="K120" s="1">
-        <v>100</v>
+        <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5415,7 +5412,7 @@
         <v>81</v>
       </c>
       <c r="E121" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>15</v>
@@ -5424,7 +5421,7 @@
         <v>16</v>
       </c>
       <c r="H121" s="1">
-        <v>30229.279999999999</v>
+        <v>36097.129999999997</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>17</v>
@@ -5433,7 +5430,7 @@
         <v>81</v>
       </c>
       <c r="K121" s="1">
-        <v>142</v>
+        <v>185</v>
       </c>
     </row>
     <row r="122" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5450,7 +5447,7 @@
         <v>81</v>
       </c>
       <c r="E122" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>15</v>
@@ -5459,7 +5456,7 @@
         <v>16</v>
       </c>
       <c r="H122" s="1">
-        <v>36097.129999999997</v>
+        <v>22703.07</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>17</v>
@@ -5468,7 +5465,7 @@
         <v>81</v>
       </c>
       <c r="K122" s="1">
-        <v>185</v>
+        <v>110</v>
       </c>
     </row>
     <row r="123" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5485,7 +5482,7 @@
         <v>81</v>
       </c>
       <c r="E123" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>15</v>
@@ -5494,7 +5491,7 @@
         <v>16</v>
       </c>
       <c r="H123" s="1">
-        <v>22703.07</v>
+        <v>30029.65</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>17</v>
@@ -5503,7 +5500,7 @@
         <v>81</v>
       </c>
       <c r="K123" s="1">
-        <v>110</v>
+        <v>134</v>
       </c>
     </row>
     <row r="124" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5520,7 +5517,7 @@
         <v>81</v>
       </c>
       <c r="E124" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>15</v>
@@ -5529,7 +5526,7 @@
         <v>16</v>
       </c>
       <c r="H124" s="1">
-        <v>30029.65</v>
+        <v>12920.73</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>17</v>
@@ -5538,7 +5535,7 @@
         <v>81</v>
       </c>
       <c r="K124" s="1">
-        <v>134</v>
+        <v>65</v>
       </c>
     </row>
     <row r="125" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5555,7 +5552,7 @@
         <v>81</v>
       </c>
       <c r="E125" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>15</v>
@@ -5564,7 +5561,7 @@
         <v>16</v>
       </c>
       <c r="H125" s="1">
-        <v>12920.73</v>
+        <v>17744.599999999999</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>17</v>
@@ -5573,7 +5570,7 @@
         <v>81</v>
       </c>
       <c r="K125" s="1">
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="126" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5590,7 +5587,7 @@
         <v>81</v>
       </c>
       <c r="E126" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>15</v>
@@ -5599,7 +5596,7 @@
         <v>16</v>
       </c>
       <c r="H126" s="1">
-        <v>17744.599999999999</v>
+        <v>38272.730000000003</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>17</v>
@@ -5608,7 +5605,7 @@
         <v>81</v>
       </c>
       <c r="K126" s="1">
-        <v>91</v>
+        <v>163</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5625,7 +5622,7 @@
         <v>81</v>
       </c>
       <c r="E127" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>15</v>
@@ -5634,16 +5631,16 @@
         <v>16</v>
       </c>
       <c r="H127" s="1">
-        <v>38272.730000000003</v>
+        <v>34006.589999999997</v>
       </c>
       <c r="I127" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="K127" s="1">
-        <v>163</v>
+        <v>187</v>
       </c>
     </row>
     <row r="128" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5660,7 +5657,7 @@
         <v>81</v>
       </c>
       <c r="E128" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>15</v>
@@ -5669,7 +5666,7 @@
         <v>16</v>
       </c>
       <c r="H128" s="1">
-        <v>34006.589999999997</v>
+        <v>28535.9</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>17</v>
@@ -5678,7 +5675,7 @@
         <v>18</v>
       </c>
       <c r="K128" s="1">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="129" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5695,7 +5692,7 @@
         <v>81</v>
       </c>
       <c r="E129" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>15</v>
@@ -5704,16 +5701,16 @@
         <v>16</v>
       </c>
       <c r="H129" s="1">
-        <v>28535.9</v>
+        <v>23919.73</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="K129" s="1">
-        <v>166</v>
+        <v>113</v>
       </c>
     </row>
     <row r="130" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5730,7 +5727,7 @@
         <v>81</v>
       </c>
       <c r="E130" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>15</v>
@@ -5739,7 +5736,7 @@
         <v>16</v>
       </c>
       <c r="H130" s="1">
-        <v>23919.73</v>
+        <v>22439.69</v>
       </c>
       <c r="I130" s="1" t="s">
         <v>17</v>
@@ -5748,7 +5745,7 @@
         <v>81</v>
       </c>
       <c r="K130" s="1">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="131" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5765,7 +5762,7 @@
         <v>81</v>
       </c>
       <c r="E131" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>15</v>
@@ -5774,7 +5771,7 @@
         <v>16</v>
       </c>
       <c r="H131" s="1">
-        <v>22439.69</v>
+        <v>20066.080000000002</v>
       </c>
       <c r="I131" s="1" t="s">
         <v>17</v>
@@ -5783,7 +5780,7 @@
         <v>81</v>
       </c>
       <c r="K131" s="1">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="132" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5800,7 +5797,7 @@
         <v>81</v>
       </c>
       <c r="E132" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>15</v>
@@ -5809,7 +5806,7 @@
         <v>16</v>
       </c>
       <c r="H132" s="1">
-        <v>20066.080000000002</v>
+        <v>23067.79</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>17</v>
@@ -5818,7 +5815,7 @@
         <v>81</v>
       </c>
       <c r="K132" s="1">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="133" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5835,7 +5832,7 @@
         <v>81</v>
       </c>
       <c r="E133" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>15</v>
@@ -5844,7 +5841,7 @@
         <v>16</v>
       </c>
       <c r="H133" s="1">
-        <v>23067.79</v>
+        <v>33416.58</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>17</v>
@@ -5853,7 +5850,7 @@
         <v>81</v>
       </c>
       <c r="K133" s="1">
-        <v>104</v>
+        <v>162</v>
       </c>
     </row>
     <row r="134" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5864,42 +5861,42 @@
         <v>10</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E134" s="1">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>15</v>
+        <v>269</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>16</v>
+        <v>270</v>
       </c>
       <c r="H134" s="1">
-        <v>33416.58</v>
+        <v>16012.17</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="K134" s="1">
-        <v>162</v>
+        <v>93</v>
       </c>
     </row>
     <row r="135" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>81</v>
@@ -5908,13 +5905,13 @@
         <v>1</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H135" s="1">
-        <v>16012.17</v>
+        <v>127197.96</v>
       </c>
       <c r="I135" s="1" t="s">
         <v>67</v>
@@ -5923,7 +5920,7 @@
         <v>68</v>
       </c>
       <c r="K135" s="1">
-        <v>93</v>
+        <v>480</v>
       </c>
     </row>
     <row r="136" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5934,22 +5931,22 @@
         <v>10</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E136" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H136" s="1">
-        <v>127197.96</v>
+        <v>24168.74</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>67</v>
@@ -5958,7 +5955,7 @@
         <v>68</v>
       </c>
       <c r="K136" s="1">
-        <v>480</v>
+        <v>187</v>
       </c>
     </row>
     <row r="137" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -5969,7 +5966,7 @@
         <v>10</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>81</v>
@@ -5978,13 +5975,13 @@
         <v>2</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H137" s="1">
-        <v>24168.74</v>
+        <v>71727.710000000006</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>67</v>
@@ -5993,7 +5990,7 @@
         <v>68</v>
       </c>
       <c r="K137" s="1">
-        <v>187</v>
+        <v>335</v>
       </c>
     </row>
     <row r="138" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6004,22 +6001,22 @@
         <v>10</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E138" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H138" s="1">
-        <v>71727.710000000006</v>
+        <v>34576.910000000003</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>67</v>
@@ -6028,7 +6025,7 @@
         <v>68</v>
       </c>
       <c r="K138" s="1">
-        <v>335</v>
+        <v>218</v>
       </c>
     </row>
     <row r="139" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6039,7 +6036,7 @@
         <v>10</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>81</v>
@@ -6048,13 +6045,13 @@
         <v>3</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H139" s="1">
-        <v>34576.910000000003</v>
+        <v>91677.759999999995</v>
       </c>
       <c r="I139" s="1" t="s">
         <v>67</v>
@@ -6063,7 +6060,7 @@
         <v>68</v>
       </c>
       <c r="K139" s="1">
-        <v>218</v>
+        <v>329</v>
       </c>
     </row>
     <row r="140" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6074,22 +6071,22 @@
         <v>10</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E140" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H140" s="1">
-        <v>91677.759999999995</v>
+        <v>29351.52</v>
       </c>
       <c r="I140" s="1" t="s">
         <v>67</v>
@@ -6098,7 +6095,7 @@
         <v>68</v>
       </c>
       <c r="K140" s="1">
-        <v>329</v>
+        <v>213</v>
       </c>
     </row>
     <row r="141" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6109,7 +6106,7 @@
         <v>10</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>81</v>
@@ -6118,13 +6115,13 @@
         <v>4</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H141" s="1">
-        <v>29351.52</v>
+        <v>85295.1</v>
       </c>
       <c r="I141" s="1" t="s">
         <v>67</v>
@@ -6133,7 +6130,7 @@
         <v>68</v>
       </c>
       <c r="K141" s="1">
-        <v>213</v>
+        <v>352</v>
       </c>
     </row>
     <row r="142" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6144,22 +6141,22 @@
         <v>10</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E142" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H142" s="1">
-        <v>85295.1</v>
+        <v>12287.31</v>
       </c>
       <c r="I142" s="1" t="s">
         <v>67</v>
@@ -6168,7 +6165,7 @@
         <v>68</v>
       </c>
       <c r="K142" s="1">
-        <v>352</v>
+        <v>84</v>
       </c>
     </row>
     <row r="143" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6179,7 +6176,7 @@
         <v>10</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>81</v>
@@ -6188,13 +6185,13 @@
         <v>5</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H143" s="1">
-        <v>12287.31</v>
+        <v>90680.26</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>67</v>
@@ -6203,7 +6200,7 @@
         <v>68</v>
       </c>
       <c r="K143" s="1">
-        <v>84</v>
+        <v>423</v>
       </c>
     </row>
     <row r="144" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6214,22 +6211,22 @@
         <v>10</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E144" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H144" s="1">
-        <v>90680.26</v>
+        <v>19644.72</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>67</v>
@@ -6238,7 +6235,7 @@
         <v>68</v>
       </c>
       <c r="K144" s="1">
-        <v>423</v>
+        <v>114</v>
       </c>
     </row>
     <row r="145" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6249,7 +6246,7 @@
         <v>10</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>81</v>
@@ -6258,13 +6255,13 @@
         <v>6</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H145" s="1">
-        <v>19644.72</v>
+        <v>56847.48</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>67</v>
@@ -6273,7 +6270,7 @@
         <v>68</v>
       </c>
       <c r="K145" s="1">
-        <v>114</v>
+        <v>251</v>
       </c>
     </row>
     <row r="146" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6284,31 +6281,31 @@
         <v>10</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E146" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>268</v>
+        <v>15</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>269</v>
+        <v>16</v>
       </c>
       <c r="H146" s="1">
-        <v>56847.48</v>
+        <v>11855.13</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="K146" s="1">
-        <v>251</v>
+        <v>88</v>
       </c>
     </row>
     <row r="147" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6319,13 +6316,13 @@
         <v>10</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E147" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>15</v>
@@ -6334,7 +6331,7 @@
         <v>16</v>
       </c>
       <c r="H147" s="1">
-        <v>11855.13</v>
+        <v>21459.78</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>17</v>
@@ -6343,7 +6340,7 @@
         <v>81</v>
       </c>
       <c r="K147" s="1">
-        <v>88</v>
+        <v>147</v>
       </c>
     </row>
     <row r="148" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6354,13 +6351,13 @@
         <v>10</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E148" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>15</v>
@@ -6369,7 +6366,7 @@
         <v>16</v>
       </c>
       <c r="H148" s="1">
-        <v>21459.78</v>
+        <v>25527.25</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>17</v>
@@ -6378,7 +6375,7 @@
         <v>81</v>
       </c>
       <c r="K148" s="1">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="149" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6389,31 +6386,31 @@
         <v>10</v>
       </c>
       <c r="C149" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E149" s="1">
+        <v>10</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H149" s="1">
+        <v>25759.32</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K149" s="1">
         <v>156</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E149" s="1">
-        <v>9</v>
-      </c>
-      <c r="F149" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G149" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H149" s="1">
-        <v>25527.25</v>
-      </c>
-      <c r="I149" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J149" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K149" s="1">
-        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6424,13 +6421,13 @@
         <v>10</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E150" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>15</v>
@@ -6439,7 +6436,7 @@
         <v>16</v>
       </c>
       <c r="H150" s="1">
-        <v>25759.32</v>
+        <v>14595.23</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>17</v>
@@ -6448,7 +6445,7 @@
         <v>81</v>
       </c>
       <c r="K150" s="1">
-        <v>156</v>
+        <v>100</v>
       </c>
     </row>
     <row r="151" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6459,13 +6456,13 @@
         <v>10</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E151" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>15</v>
@@ -6474,7 +6471,7 @@
         <v>16</v>
       </c>
       <c r="H151" s="1">
-        <v>14595.23</v>
+        <v>18690.46</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>17</v>
@@ -6483,7 +6480,7 @@
         <v>81</v>
       </c>
       <c r="K151" s="1">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="152" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6494,13 +6491,13 @@
         <v>10</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E152" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>15</v>
@@ -6509,16 +6506,16 @@
         <v>16</v>
       </c>
       <c r="H152" s="1">
-        <v>18690.46</v>
+        <v>21113.94</v>
       </c>
       <c r="I152" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="K152" s="1">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6529,13 +6526,13 @@
         <v>10</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E153" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>15</v>
@@ -6544,7 +6541,7 @@
         <v>16</v>
       </c>
       <c r="H153" s="1">
-        <v>21113.94</v>
+        <v>18368.830000000002</v>
       </c>
       <c r="I153" s="1" t="s">
         <v>17</v>
@@ -6553,7 +6550,7 @@
         <v>18</v>
       </c>
       <c r="K153" s="1">
-        <v>136</v>
+        <v>96</v>
       </c>
     </row>
     <row r="154" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6564,13 +6561,13 @@
         <v>10</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E154" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>15</v>
@@ -6579,7 +6576,7 @@
         <v>16</v>
       </c>
       <c r="H154" s="1">
-        <v>18368.830000000002</v>
+        <v>17547.88</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>17</v>
@@ -6588,7 +6585,7 @@
         <v>18</v>
       </c>
       <c r="K154" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="155" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6599,13 +6596,13 @@
         <v>10</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E155" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>15</v>
@@ -6614,7 +6611,7 @@
         <v>16</v>
       </c>
       <c r="H155" s="1">
-        <v>17547.88</v>
+        <v>14923.97</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>17</v>
@@ -6623,7 +6620,7 @@
         <v>18</v>
       </c>
       <c r="K155" s="1">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="156" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6634,13 +6631,13 @@
         <v>10</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E156" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>15</v>
@@ -6649,7 +6646,7 @@
         <v>16</v>
       </c>
       <c r="H156" s="1">
-        <v>14923.97</v>
+        <v>14750.32</v>
       </c>
       <c r="I156" s="1" t="s">
         <v>17</v>
@@ -6658,7 +6655,7 @@
         <v>18</v>
       </c>
       <c r="K156" s="1">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="157" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6669,31 +6666,31 @@
         <v>10</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E157" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>15</v>
+        <v>269</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>16</v>
+        <v>270</v>
       </c>
       <c r="H157" s="1">
-        <v>14750.32</v>
+        <v>22152.11</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="K157" s="1">
-        <v>100</v>
+        <v>183</v>
       </c>
     </row>
     <row r="158" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6713,13 +6710,13 @@
         <v>1</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H158" s="1">
-        <v>22152.11</v>
+        <v>71817.919999999998</v>
       </c>
       <c r="I158" s="1" t="s">
         <v>67</v>
@@ -6728,7 +6725,7 @@
         <v>68</v>
       </c>
       <c r="K158" s="1">
-        <v>183</v>
+        <v>421</v>
       </c>
     </row>
     <row r="159" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6745,16 +6742,16 @@
         <v>14</v>
       </c>
       <c r="E159" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H159" s="1">
-        <v>71817.919999999998</v>
+        <v>37316.699999999997</v>
       </c>
       <c r="I159" s="1" t="s">
         <v>67</v>
@@ -6763,7 +6760,7 @@
         <v>68</v>
       </c>
       <c r="K159" s="1">
-        <v>421</v>
+        <v>323</v>
       </c>
     </row>
     <row r="160" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6783,13 +6780,13 @@
         <v>2</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H160" s="1">
-        <v>37316.699999999997</v>
+        <v>102112.73</v>
       </c>
       <c r="I160" s="1" t="s">
         <v>67</v>
@@ -6798,7 +6795,7 @@
         <v>68</v>
       </c>
       <c r="K160" s="1">
-        <v>323</v>
+        <v>565</v>
       </c>
     </row>
     <row r="161" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6815,16 +6812,16 @@
         <v>14</v>
       </c>
       <c r="E161" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H161" s="1">
-        <v>102112.73</v>
+        <v>18398.689999999999</v>
       </c>
       <c r="I161" s="1" t="s">
         <v>67</v>
@@ -6833,7 +6830,7 @@
         <v>68</v>
       </c>
       <c r="K161" s="1">
-        <v>565</v>
+        <v>162</v>
       </c>
     </row>
     <row r="162" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6853,13 +6850,13 @@
         <v>3</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H162" s="1">
-        <v>18398.689999999999</v>
+        <v>85148.24</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>67</v>
@@ -6868,7 +6865,7 @@
         <v>68</v>
       </c>
       <c r="K162" s="1">
-        <v>162</v>
+        <v>490</v>
       </c>
     </row>
     <row r="163" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6885,16 +6882,16 @@
         <v>14</v>
       </c>
       <c r="E163" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H163" s="1">
-        <v>85148.24</v>
+        <v>34778.480000000003</v>
       </c>
       <c r="I163" s="1" t="s">
         <v>67</v>
@@ -6903,7 +6900,7 @@
         <v>68</v>
       </c>
       <c r="K163" s="1">
-        <v>490</v>
+        <v>293</v>
       </c>
     </row>
     <row r="164" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6923,13 +6920,13 @@
         <v>4</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H164" s="1">
-        <v>34778.480000000003</v>
+        <v>87237.5</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>67</v>
@@ -6938,7 +6935,7 @@
         <v>68</v>
       </c>
       <c r="K164" s="1">
-        <v>293</v>
+        <v>758</v>
       </c>
     </row>
     <row r="165" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6955,16 +6952,16 @@
         <v>14</v>
       </c>
       <c r="E165" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H165" s="1">
-        <v>87237.5</v>
+        <v>23435.74</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>67</v>
@@ -6973,7 +6970,7 @@
         <v>68</v>
       </c>
       <c r="K165" s="1">
-        <v>758</v>
+        <v>201</v>
       </c>
     </row>
     <row r="166" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -6993,13 +6990,13 @@
         <v>5</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H166" s="1">
-        <v>23435.74</v>
+        <v>78840.789999999994</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>67</v>
@@ -7008,7 +7005,7 @@
         <v>68</v>
       </c>
       <c r="K166" s="1">
-        <v>201</v>
+        <v>714</v>
       </c>
     </row>
     <row r="167" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7025,16 +7022,16 @@
         <v>14</v>
       </c>
       <c r="E167" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H167" s="1">
-        <v>78840.789999999994</v>
+        <v>25414.45</v>
       </c>
       <c r="I167" s="1" t="s">
         <v>67</v>
@@ -7043,7 +7040,7 @@
         <v>68</v>
       </c>
       <c r="K167" s="1">
-        <v>714</v>
+        <v>211</v>
       </c>
     </row>
     <row r="168" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7063,13 +7060,13 @@
         <v>6</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H168" s="1">
-        <v>25414.45</v>
+        <v>102140.65</v>
       </c>
       <c r="I168" s="1" t="s">
         <v>67</v>
@@ -7078,7 +7075,7 @@
         <v>68</v>
       </c>
       <c r="K168" s="1">
-        <v>211</v>
+        <v>612</v>
       </c>
     </row>
     <row r="169" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7089,32 +7086,16 @@
         <v>10</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D169" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E169" s="1">
-        <v>6</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G169" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="H169" s="1">
-        <v>102140.65</v>
-      </c>
-      <c r="I169" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J169" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K169" s="1">
-        <v>612</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1"/>
+      <c r="I169" s="1"/>
+      <c r="J169" s="1"/>
+      <c r="K169" s="1"/>
     </row>
     <row r="170" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
@@ -7124,32 +7105,48 @@
         <v>10</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D170" s="1"/>
-      <c r="E170" s="1"/>
-      <c r="F170" s="1"/>
-      <c r="G170" s="1"/>
-      <c r="H170" s="1"/>
-      <c r="I170" s="1"/>
-      <c r="J170" s="1"/>
-      <c r="K170" s="1"/>
+        <v>192</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E170" s="1">
+        <v>15</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H170" s="1">
+        <v>17343.439999999999</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J170" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K170" s="1">
+        <v>103</v>
+      </c>
     </row>
     <row r="171" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B171" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="D171" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E171" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>15</v>
@@ -7158,7 +7155,7 @@
         <v>16</v>
       </c>
       <c r="H171" s="1">
-        <v>17343.439999999999</v>
+        <v>27363.79</v>
       </c>
       <c r="I171" s="1" t="s">
         <v>17</v>
@@ -7167,7 +7164,7 @@
         <v>81</v>
       </c>
       <c r="K171" s="1">
-        <v>103</v>
+        <v>196</v>
       </c>
     </row>
     <row r="172" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7178,13 +7175,13 @@
         <v>10</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E172" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>15</v>
@@ -7193,7 +7190,7 @@
         <v>16</v>
       </c>
       <c r="H172" s="1">
-        <v>27363.79</v>
+        <v>21838.18</v>
       </c>
       <c r="I172" s="1" t="s">
         <v>17</v>
@@ -7202,7 +7199,7 @@
         <v>81</v>
       </c>
       <c r="K172" s="1">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="173" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7213,13 +7210,13 @@
         <v>10</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E173" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>15</v>
@@ -7228,7 +7225,7 @@
         <v>16</v>
       </c>
       <c r="H173" s="1">
-        <v>21838.18</v>
+        <v>29316.19</v>
       </c>
       <c r="I173" s="1" t="s">
         <v>17</v>
@@ -7237,7 +7234,7 @@
         <v>81</v>
       </c>
       <c r="K173" s="1">
-        <v>159</v>
+        <v>224</v>
       </c>
     </row>
     <row r="174" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7248,31 +7245,31 @@
         <v>10</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E174" s="1">
+        <v>19</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H174" s="1">
+        <v>23376.82</v>
+      </c>
+      <c r="I174" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J174" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F174" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G174" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H174" s="1">
-        <v>29316.19</v>
-      </c>
-      <c r="I174" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J174" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="K174" s="1">
-        <v>224</v>
+        <v>130</v>
       </c>
     </row>
     <row r="175" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7283,13 +7280,13 @@
         <v>10</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E175" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>15</v>
@@ -7298,7 +7295,7 @@
         <v>16</v>
       </c>
       <c r="H175" s="1">
-        <v>23376.82</v>
+        <v>34871.379999999997</v>
       </c>
       <c r="I175" s="1" t="s">
         <v>17</v>
@@ -7307,7 +7304,7 @@
         <v>18</v>
       </c>
       <c r="K175" s="1">
-        <v>130</v>
+        <v>185</v>
       </c>
     </row>
     <row r="176" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7318,13 +7315,13 @@
         <v>10</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E176" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>15</v>
@@ -7333,7 +7330,7 @@
         <v>16</v>
       </c>
       <c r="H176" s="1">
-        <v>34871.379999999997</v>
+        <v>29638.5</v>
       </c>
       <c r="I176" s="1" t="s">
         <v>17</v>
@@ -7342,7 +7339,7 @@
         <v>18</v>
       </c>
       <c r="K176" s="1">
-        <v>185</v>
+        <v>167</v>
       </c>
     </row>
     <row r="177" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7353,13 +7350,13 @@
         <v>10</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E177" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>15</v>
@@ -7368,7 +7365,7 @@
         <v>16</v>
       </c>
       <c r="H177" s="1">
-        <v>29638.5</v>
+        <v>24203.53</v>
       </c>
       <c r="I177" s="1" t="s">
         <v>17</v>
@@ -7377,7 +7374,7 @@
         <v>18</v>
       </c>
       <c r="K177" s="1">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
     <row r="178" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7388,13 +7385,13 @@
         <v>10</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E178" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>15</v>
@@ -7403,7 +7400,7 @@
         <v>16</v>
       </c>
       <c r="H178" s="1">
-        <v>24203.53</v>
+        <v>24850.07</v>
       </c>
       <c r="I178" s="1" t="s">
         <v>17</v>
@@ -7412,7 +7409,7 @@
         <v>18</v>
       </c>
       <c r="K178" s="1">
-        <v>145</v>
+        <v>162</v>
       </c>
     </row>
     <row r="179" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7423,13 +7420,13 @@
         <v>10</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E179" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>15</v>
@@ -7438,7 +7435,7 @@
         <v>16</v>
       </c>
       <c r="H179" s="1">
-        <v>24850.07</v>
+        <v>22985.599999999999</v>
       </c>
       <c r="I179" s="1" t="s">
         <v>17</v>
@@ -7447,42 +7444,42 @@
         <v>18</v>
       </c>
       <c r="K179" s="1">
-        <v>162</v>
+        <v>126</v>
       </c>
     </row>
     <row r="180" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C180" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B180" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="D180" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E180" s="1">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>15</v>
+        <v>269</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>16</v>
+        <v>270</v>
       </c>
       <c r="H180" s="1">
-        <v>22985.599999999999</v>
+        <v>11634.61</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="J180" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="K180" s="1">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="181" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7493,7 +7490,7 @@
         <v>10</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>14</v>
@@ -7502,13 +7499,13 @@
         <v>6</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H181" s="1">
-        <v>11634.61</v>
+        <v>74251.72</v>
       </c>
       <c r="I181" s="1" t="s">
         <v>67</v>
@@ -7517,7 +7514,7 @@
         <v>68</v>
       </c>
       <c r="K181" s="1">
-        <v>118</v>
+        <v>269</v>
       </c>
     </row>
     <row r="182" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7528,22 +7525,22 @@
         <v>10</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E182" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H182" s="1">
-        <v>74251.72</v>
+        <v>17370.78</v>
       </c>
       <c r="I182" s="1" t="s">
         <v>67</v>
@@ -7552,7 +7549,7 @@
         <v>68</v>
       </c>
       <c r="K182" s="1">
-        <v>269</v>
+        <v>133</v>
       </c>
     </row>
     <row r="183" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7563,7 +7560,7 @@
         <v>10</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>14</v>
@@ -7572,13 +7569,13 @@
         <v>7</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H183" s="1">
-        <v>17370.78</v>
+        <v>81639.25</v>
       </c>
       <c r="I183" s="1" t="s">
         <v>67</v>
@@ -7587,7 +7584,7 @@
         <v>68</v>
       </c>
       <c r="K183" s="1">
-        <v>133</v>
+        <v>216</v>
       </c>
     </row>
     <row r="184" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7598,22 +7595,22 @@
         <v>10</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E184" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H184" s="1">
-        <v>81639.25</v>
+        <v>10375.91</v>
       </c>
       <c r="I184" s="1" t="s">
         <v>67</v>
@@ -7622,7 +7619,7 @@
         <v>68</v>
       </c>
       <c r="K184" s="1">
-        <v>216</v>
+        <v>78</v>
       </c>
     </row>
     <row r="185" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7633,7 +7630,7 @@
         <v>10</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>14</v>
@@ -7642,13 +7639,13 @@
         <v>8</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H185" s="1">
-        <v>10375.91</v>
+        <v>73735.649999999994</v>
       </c>
       <c r="I185" s="1" t="s">
         <v>67</v>
@@ -7657,7 +7654,7 @@
         <v>68</v>
       </c>
       <c r="K185" s="1">
-        <v>78</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7668,22 +7665,22 @@
         <v>10</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E186" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H186" s="1">
-        <v>73735.649999999994</v>
+        <v>6450.01</v>
       </c>
       <c r="I186" s="1" t="s">
         <v>67</v>
@@ -7692,7 +7689,7 @@
         <v>68</v>
       </c>
       <c r="K186" s="1">
-        <v>187</v>
+        <v>38</v>
       </c>
     </row>
     <row r="187" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7703,7 +7700,7 @@
         <v>10</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>14</v>
@@ -7712,13 +7709,13 @@
         <v>9</v>
       </c>
       <c r="F187" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H187" s="1">
-        <v>6450.01</v>
+        <v>68227.62</v>
       </c>
       <c r="I187" s="1" t="s">
         <v>67</v>
@@ -7727,7 +7724,7 @@
         <v>68</v>
       </c>
       <c r="K187" s="1">
-        <v>38</v>
+        <v>208</v>
       </c>
     </row>
     <row r="188" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7738,22 +7735,22 @@
         <v>10</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E188" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H188" s="1">
-        <v>68227.62</v>
+        <v>12227.75</v>
       </c>
       <c r="I188" s="1" t="s">
         <v>67</v>
@@ -7762,7 +7759,7 @@
         <v>68</v>
       </c>
       <c r="K188" s="1">
-        <v>208</v>
+        <v>110</v>
       </c>
     </row>
     <row r="189" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7773,7 +7770,7 @@
         <v>10</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>14</v>
@@ -7782,13 +7779,13 @@
         <v>10</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H189" s="1">
-        <v>12227.75</v>
+        <v>78998.740000000005</v>
       </c>
       <c r="I189" s="1" t="s">
         <v>67</v>
@@ -7797,7 +7794,7 @@
         <v>68</v>
       </c>
       <c r="K189" s="1">
-        <v>110</v>
+        <v>276</v>
       </c>
     </row>
     <row r="190" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7808,22 +7805,22 @@
         <v>10</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E190" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H190" s="1">
-        <v>78998.740000000005</v>
+        <v>10457.450000000001</v>
       </c>
       <c r="I190" s="1" t="s">
         <v>67</v>
@@ -7832,7 +7829,7 @@
         <v>68</v>
       </c>
       <c r="K190" s="1">
-        <v>276</v>
+        <v>65</v>
       </c>
     </row>
     <row r="191" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7843,7 +7840,7 @@
         <v>10</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>14</v>
@@ -7852,13 +7849,13 @@
         <v>11</v>
       </c>
       <c r="F191" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H191" s="1">
-        <v>10457.450000000001</v>
+        <v>46423.18</v>
       </c>
       <c r="I191" s="1" t="s">
         <v>67</v>
@@ -7867,7 +7864,7 @@
         <v>68</v>
       </c>
       <c r="K191" s="1">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="192" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7878,31 +7875,31 @@
         <v>10</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E192" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>268</v>
+        <v>15</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>269</v>
+        <v>16</v>
       </c>
       <c r="H192" s="1">
-        <v>46423.18</v>
+        <v>23068.74</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="J192" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="K192" s="1">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="193" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7913,13 +7910,13 @@
         <v>10</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E193" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>15</v>
@@ -7928,7 +7925,7 @@
         <v>16</v>
       </c>
       <c r="H193" s="1">
-        <v>23068.74</v>
+        <v>23724.39</v>
       </c>
       <c r="I193" s="1" t="s">
         <v>17</v>
@@ -7937,7 +7934,7 @@
         <v>81</v>
       </c>
       <c r="K193" s="1">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="194" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7948,13 +7945,13 @@
         <v>10</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E194" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>15</v>
@@ -7963,7 +7960,7 @@
         <v>16</v>
       </c>
       <c r="H194" s="1">
-        <v>23724.39</v>
+        <v>15825.42</v>
       </c>
       <c r="I194" s="1" t="s">
         <v>17</v>
@@ -7972,7 +7969,7 @@
         <v>81</v>
       </c>
       <c r="K194" s="1">
-        <v>132</v>
+        <v>89</v>
       </c>
     </row>
     <row r="195" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -7983,13 +7980,13 @@
         <v>10</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E195" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>15</v>
@@ -7998,7 +7995,7 @@
         <v>16</v>
       </c>
       <c r="H195" s="1">
-        <v>15825.42</v>
+        <v>23053.23</v>
       </c>
       <c r="I195" s="1" t="s">
         <v>17</v>
@@ -8007,7 +8004,7 @@
         <v>81</v>
       </c>
       <c r="K195" s="1">
-        <v>89</v>
+        <v>125</v>
       </c>
     </row>
     <row r="196" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8018,13 +8015,13 @@
         <v>10</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E196" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>15</v>
@@ -8033,7 +8030,7 @@
         <v>16</v>
       </c>
       <c r="H196" s="1">
-        <v>23053.23</v>
+        <v>18840.2</v>
       </c>
       <c r="I196" s="1" t="s">
         <v>17</v>
@@ -8042,7 +8039,7 @@
         <v>81</v>
       </c>
       <c r="K196" s="1">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="197" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8053,13 +8050,13 @@
         <v>10</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E197" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>15</v>
@@ -8068,7 +8065,7 @@
         <v>16</v>
       </c>
       <c r="H197" s="1">
-        <v>18840.2</v>
+        <v>15928.86</v>
       </c>
       <c r="I197" s="1" t="s">
         <v>17</v>
@@ -8077,7 +8074,7 @@
         <v>81</v>
       </c>
       <c r="K197" s="1">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
     <row r="198" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8088,13 +8085,13 @@
         <v>10</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E198" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>15</v>
@@ -8103,16 +8100,16 @@
         <v>16</v>
       </c>
       <c r="H198" s="1">
-        <v>15928.86</v>
+        <v>24020</v>
       </c>
       <c r="I198" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J198" s="1" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
       <c r="K198" s="1">
-        <v>82</v>
+        <v>131</v>
       </c>
     </row>
     <row r="199" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8123,13 +8120,13 @@
         <v>10</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E199" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>15</v>
@@ -8138,7 +8135,7 @@
         <v>16</v>
       </c>
       <c r="H199" s="1">
-        <v>24020</v>
+        <v>30831.81</v>
       </c>
       <c r="I199" s="1" t="s">
         <v>17</v>
@@ -8147,7 +8144,7 @@
         <v>18</v>
       </c>
       <c r="K199" s="1">
-        <v>131</v>
+        <v>155</v>
       </c>
     </row>
     <row r="200" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8158,13 +8155,13 @@
         <v>10</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E200" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>15</v>
@@ -8173,7 +8170,7 @@
         <v>16</v>
       </c>
       <c r="H200" s="1">
-        <v>30831.81</v>
+        <v>25241.13</v>
       </c>
       <c r="I200" s="1" t="s">
         <v>17</v>
@@ -8182,7 +8179,7 @@
         <v>18</v>
       </c>
       <c r="K200" s="1">
-        <v>155</v>
+        <v>133</v>
       </c>
     </row>
     <row r="201" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8193,13 +8190,13 @@
         <v>10</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E201" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>15</v>
@@ -8208,7 +8205,7 @@
         <v>16</v>
       </c>
       <c r="H201" s="1">
-        <v>25241.13</v>
+        <v>20817.849999999999</v>
       </c>
       <c r="I201" s="1" t="s">
         <v>17</v>
@@ -8217,7 +8214,7 @@
         <v>18</v>
       </c>
       <c r="K201" s="1">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="202" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8228,13 +8225,13 @@
         <v>10</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E202" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>15</v>
@@ -8243,7 +8240,7 @@
         <v>16</v>
       </c>
       <c r="H202" s="1">
-        <v>20817.849999999999</v>
+        <v>37763.21</v>
       </c>
       <c r="I202" s="1" t="s">
         <v>17</v>
@@ -8252,7 +8249,7 @@
         <v>18</v>
       </c>
       <c r="K202" s="1">
-        <v>124</v>
+        <v>184</v>
       </c>
     </row>
     <row r="203" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8263,13 +8260,13 @@
         <v>10</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E203" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>15</v>
@@ -8278,7 +8275,7 @@
         <v>16</v>
       </c>
       <c r="H203" s="1">
-        <v>37763.21</v>
+        <v>35559.96</v>
       </c>
       <c r="I203" s="1" t="s">
         <v>17</v>
@@ -8287,7 +8284,7 @@
         <v>18</v>
       </c>
       <c r="K203" s="1">
-        <v>184</v>
+        <v>203</v>
       </c>
     </row>
     <row r="204" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8298,51 +8295,51 @@
         <v>10</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D204" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E204" s="1">
-        <v>23</v>
-      </c>
-      <c r="F204" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G204" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H204" s="1">
-        <v>35559.96</v>
-      </c>
-      <c r="I204" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J204" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K204" s="1">
-        <v>203</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D204" s="1"/>
+      <c r="E204" s="1"/>
+      <c r="F204" s="1"/>
+      <c r="G204" s="1"/>
+      <c r="H204" s="1"/>
+      <c r="I204" s="1"/>
+      <c r="J204" s="1"/>
+      <c r="K204" s="1"/>
     </row>
     <row r="205" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C205" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B205" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D205" s="1"/>
-      <c r="E205" s="1"/>
-      <c r="F205" s="1"/>
-      <c r="G205" s="1"/>
-      <c r="H205" s="1"/>
-      <c r="I205" s="1"/>
-      <c r="J205" s="1"/>
-      <c r="K205" s="1"/>
+      <c r="D205" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E205" s="1">
+        <v>7</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G205" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H205" s="1">
+        <v>8313.84</v>
+      </c>
+      <c r="I205" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J205" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K205" s="1">
+        <v>64</v>
+      </c>
     </row>
     <row r="206" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
@@ -8352,7 +8349,7 @@
         <v>10</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>81</v>
@@ -8361,13 +8358,13 @@
         <v>7</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H206" s="1">
-        <v>8313.84</v>
+        <v>96174.64</v>
       </c>
       <c r="I206" s="1" t="s">
         <v>67</v>
@@ -8376,7 +8373,7 @@
         <v>68</v>
       </c>
       <c r="K206" s="1">
-        <v>64</v>
+        <v>295</v>
       </c>
     </row>
     <row r="207" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8387,22 +8384,22 @@
         <v>10</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E207" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H207" s="1">
-        <v>96174.64</v>
+        <v>6364.16</v>
       </c>
       <c r="I207" s="1" t="s">
         <v>67</v>
@@ -8411,7 +8408,7 @@
         <v>68</v>
       </c>
       <c r="K207" s="1">
-        <v>295</v>
+        <v>49</v>
       </c>
     </row>
     <row r="208" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8422,7 +8419,7 @@
         <v>10</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>81</v>
@@ -8431,13 +8428,13 @@
         <v>8</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H208" s="1">
-        <v>6364.16</v>
+        <v>60662.64</v>
       </c>
       <c r="I208" s="1" t="s">
         <v>67</v>
@@ -8446,7 +8443,7 @@
         <v>68</v>
       </c>
       <c r="K208" s="1">
-        <v>49</v>
+        <v>177</v>
       </c>
     </row>
     <row r="209" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8457,22 +8454,22 @@
         <v>10</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E209" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H209" s="1">
-        <v>60662.64</v>
+        <v>21252.87</v>
       </c>
       <c r="I209" s="1" t="s">
         <v>67</v>
@@ -8481,7 +8478,7 @@
         <v>68</v>
       </c>
       <c r="K209" s="1">
-        <v>177</v>
+        <v>155</v>
       </c>
     </row>
     <row r="210" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8492,7 +8489,7 @@
         <v>10</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>81</v>
@@ -8501,13 +8498,13 @@
         <v>9</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H210" s="1">
-        <v>21252.87</v>
+        <v>85405.91</v>
       </c>
       <c r="I210" s="1" t="s">
         <v>67</v>
@@ -8516,7 +8513,7 @@
         <v>68</v>
       </c>
       <c r="K210" s="1">
-        <v>155</v>
+        <v>352</v>
       </c>
     </row>
     <row r="211" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8527,22 +8524,22 @@
         <v>10</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E211" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H211" s="1">
-        <v>85405.91</v>
+        <v>7349.79</v>
       </c>
       <c r="I211" s="1" t="s">
         <v>67</v>
@@ -8551,7 +8548,7 @@
         <v>68</v>
       </c>
       <c r="K211" s="1">
-        <v>352</v>
+        <v>60</v>
       </c>
     </row>
     <row r="212" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8562,7 +8559,7 @@
         <v>10</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>81</v>
@@ -8571,13 +8568,13 @@
         <v>10</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H212" s="1">
-        <v>7349.79</v>
+        <v>66892.02</v>
       </c>
       <c r="I212" s="1" t="s">
         <v>67</v>
@@ -8586,7 +8583,7 @@
         <v>68</v>
       </c>
       <c r="K212" s="1">
-        <v>60</v>
+        <v>200</v>
       </c>
     </row>
     <row r="213" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8597,22 +8594,22 @@
         <v>10</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E213" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H213" s="1">
-        <v>66892.02</v>
+        <v>11468.34</v>
       </c>
       <c r="I213" s="1" t="s">
         <v>67</v>
@@ -8621,7 +8618,7 @@
         <v>68</v>
       </c>
       <c r="K213" s="1">
-        <v>200</v>
+        <v>93</v>
       </c>
     </row>
     <row r="214" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8632,7 +8629,7 @@
         <v>10</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>81</v>
@@ -8641,13 +8638,13 @@
         <v>11</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H214" s="1">
-        <v>11468.34</v>
+        <v>118494.68</v>
       </c>
       <c r="I214" s="1" t="s">
         <v>67</v>
@@ -8656,7 +8653,7 @@
         <v>68</v>
       </c>
       <c r="K214" s="1">
-        <v>93</v>
+        <v>412</v>
       </c>
     </row>
     <row r="215" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8667,22 +8664,22 @@
         <v>10</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E215" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H215" s="1">
-        <v>118494.68</v>
+        <v>12457.97</v>
       </c>
       <c r="I215" s="1" t="s">
         <v>67</v>
@@ -8691,7 +8688,7 @@
         <v>68</v>
       </c>
       <c r="K215" s="1">
-        <v>412</v>
+        <v>106</v>
       </c>
     </row>
     <row r="216" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8702,7 +8699,7 @@
         <v>10</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>81</v>
@@ -8711,13 +8708,13 @@
         <v>12</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H216" s="1">
-        <v>12457.97</v>
+        <v>160617.85</v>
       </c>
       <c r="I216" s="1" t="s">
         <v>67</v>
@@ -8726,7 +8723,7 @@
         <v>68</v>
       </c>
       <c r="K216" s="1">
-        <v>106</v>
+        <v>407</v>
       </c>
     </row>
     <row r="217" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8737,31 +8734,31 @@
         <v>10</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E217" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F217" s="1" t="s">
-        <v>268</v>
+        <v>15</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>269</v>
+        <v>16</v>
       </c>
       <c r="H217" s="1">
-        <v>160617.85</v>
+        <v>24103.13</v>
       </c>
       <c r="I217" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="J217" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="K217" s="1">
-        <v>407</v>
+        <v>151</v>
       </c>
     </row>
     <row r="218" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8772,13 +8769,13 @@
         <v>10</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E218" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>15</v>
@@ -8787,7 +8784,7 @@
         <v>16</v>
       </c>
       <c r="H218" s="1">
-        <v>24103.13</v>
+        <v>25156.07</v>
       </c>
       <c r="I218" s="1" t="s">
         <v>17</v>
@@ -8796,7 +8793,7 @@
         <v>81</v>
       </c>
       <c r="K218" s="1">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="219" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8807,13 +8804,13 @@
         <v>10</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E219" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>15</v>
@@ -8822,7 +8819,7 @@
         <v>16</v>
       </c>
       <c r="H219" s="1">
-        <v>25156.07</v>
+        <v>22744.19</v>
       </c>
       <c r="I219" s="1" t="s">
         <v>17</v>
@@ -8831,7 +8828,7 @@
         <v>81</v>
       </c>
       <c r="K219" s="1">
-        <v>161</v>
+        <v>118</v>
       </c>
     </row>
     <row r="220" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8842,13 +8839,13 @@
         <v>10</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E220" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>15</v>
@@ -8857,7 +8854,7 @@
         <v>16</v>
       </c>
       <c r="H220" s="1">
-        <v>22744.19</v>
+        <v>25428.34</v>
       </c>
       <c r="I220" s="1" t="s">
         <v>17</v>
@@ -8866,7 +8863,7 @@
         <v>81</v>
       </c>
       <c r="K220" s="1">
-        <v>118</v>
+        <v>138</v>
       </c>
     </row>
     <row r="221" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8877,13 +8874,13 @@
         <v>10</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E221" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>15</v>
@@ -8892,7 +8889,7 @@
         <v>16</v>
       </c>
       <c r="H221" s="1">
-        <v>25428.34</v>
+        <v>23616.15</v>
       </c>
       <c r="I221" s="1" t="s">
         <v>17</v>
@@ -8901,7 +8898,7 @@
         <v>81</v>
       </c>
       <c r="K221" s="1">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="222" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8912,13 +8909,13 @@
         <v>10</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E222" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>15</v>
@@ -8927,7 +8924,7 @@
         <v>16</v>
       </c>
       <c r="H222" s="1">
-        <v>23616.15</v>
+        <v>19466.75</v>
       </c>
       <c r="I222" s="1" t="s">
         <v>17</v>
@@ -8936,7 +8933,7 @@
         <v>81</v>
       </c>
       <c r="K222" s="1">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="223" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8947,31 +8944,31 @@
         <v>10</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E223" s="1">
+        <v>19</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G223" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H223" s="1">
+        <v>26072</v>
+      </c>
+      <c r="I223" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J223" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F223" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G223" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H223" s="1">
-        <v>19466.75</v>
-      </c>
-      <c r="I223" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J223" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="K223" s="1">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="224" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -8982,13 +8979,13 @@
         <v>10</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E224" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>15</v>
@@ -8997,7 +8994,7 @@
         <v>16</v>
       </c>
       <c r="H224" s="1">
-        <v>26072</v>
+        <v>17504.12</v>
       </c>
       <c r="I224" s="1" t="s">
         <v>17</v>
@@ -9006,7 +9003,7 @@
         <v>18</v>
       </c>
       <c r="K224" s="1">
-        <v>139</v>
+        <v>89</v>
       </c>
     </row>
     <row r="225" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9017,13 +9014,13 @@
         <v>10</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E225" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>15</v>
@@ -9032,7 +9029,7 @@
         <v>16</v>
       </c>
       <c r="H225" s="1">
-        <v>17504.12</v>
+        <v>14347.54</v>
       </c>
       <c r="I225" s="1" t="s">
         <v>17</v>
@@ -9041,7 +9038,7 @@
         <v>18</v>
       </c>
       <c r="K225" s="1">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="226" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9052,13 +9049,13 @@
         <v>10</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E226" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>15</v>
@@ -9067,7 +9064,7 @@
         <v>16</v>
       </c>
       <c r="H226" s="1">
-        <v>14347.54</v>
+        <v>18453.14</v>
       </c>
       <c r="I226" s="1" t="s">
         <v>17</v>
@@ -9076,7 +9073,7 @@
         <v>18</v>
       </c>
       <c r="K226" s="1">
-        <v>76</v>
+        <v>129</v>
       </c>
     </row>
     <row r="227" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9087,31 +9084,31 @@
         <v>10</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="E227" s="1">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F227" s="1" t="s">
-        <v>15</v>
+        <v>269</v>
       </c>
       <c r="G227" s="1" t="s">
-        <v>16</v>
+        <v>270</v>
       </c>
       <c r="H227" s="1">
-        <v>18453.14</v>
+        <v>11510.39</v>
       </c>
       <c r="I227" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="J227" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="K227" s="1">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="228" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9122,7 +9119,7 @@
         <v>10</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>14</v>
@@ -9131,13 +9128,13 @@
         <v>7</v>
       </c>
       <c r="F228" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G228" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H228" s="1">
-        <v>11510.39</v>
+        <v>61035.47</v>
       </c>
       <c r="I228" s="1" t="s">
         <v>67</v>
@@ -9146,7 +9143,7 @@
         <v>68</v>
       </c>
       <c r="K228" s="1">
-        <v>115</v>
+        <v>289</v>
       </c>
     </row>
     <row r="229" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9157,22 +9154,22 @@
         <v>10</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D229" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E229" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G229" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H229" s="1">
-        <v>61035.47</v>
+        <v>10672.48</v>
       </c>
       <c r="I229" s="1" t="s">
         <v>67</v>
@@ -9181,7 +9178,7 @@
         <v>68</v>
       </c>
       <c r="K229" s="1">
-        <v>289</v>
+        <v>114</v>
       </c>
     </row>
     <row r="230" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9192,7 +9189,7 @@
         <v>10</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D230" s="3" t="s">
         <v>14</v>
@@ -9201,13 +9198,13 @@
         <v>8</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G230" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H230" s="1">
-        <v>10672.48</v>
+        <v>70102.8</v>
       </c>
       <c r="I230" s="1" t="s">
         <v>67</v>
@@ -9216,7 +9213,7 @@
         <v>68</v>
       </c>
       <c r="K230" s="1">
-        <v>114</v>
+        <v>239</v>
       </c>
     </row>
     <row r="231" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9227,22 +9224,22 @@
         <v>10</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D231" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E231" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F231" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G231" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H231" s="1">
-        <v>70102.8</v>
+        <v>15331.41</v>
       </c>
       <c r="I231" s="1" t="s">
         <v>67</v>
@@ -9251,7 +9248,7 @@
         <v>68</v>
       </c>
       <c r="K231" s="1">
-        <v>239</v>
+        <v>131</v>
       </c>
     </row>
     <row r="232" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9262,7 +9259,7 @@
         <v>10</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>14</v>
@@ -9271,13 +9268,13 @@
         <v>9</v>
       </c>
       <c r="F232" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G232" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H232" s="1">
-        <v>15331.41</v>
+        <v>120199.59</v>
       </c>
       <c r="I232" s="1" t="s">
         <v>67</v>
@@ -9286,7 +9283,7 @@
         <v>68</v>
       </c>
       <c r="K232" s="1">
-        <v>131</v>
+        <v>384</v>
       </c>
     </row>
     <row r="233" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9297,22 +9294,22 @@
         <v>10</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D233" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E233" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G233" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H233" s="1">
-        <v>120199.59</v>
+        <v>24825.61</v>
       </c>
       <c r="I233" s="1" t="s">
         <v>67</v>
@@ -9321,7 +9318,7 @@
         <v>68</v>
       </c>
       <c r="K233" s="1">
-        <v>384</v>
+        <v>225</v>
       </c>
     </row>
     <row r="234" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9332,7 +9329,7 @@
         <v>10</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>14</v>
@@ -9341,13 +9338,13 @@
         <v>10</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G234" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H234" s="1">
-        <v>24825.61</v>
+        <v>184639.44</v>
       </c>
       <c r="I234" s="1" t="s">
         <v>67</v>
@@ -9356,7 +9353,7 @@
         <v>68</v>
       </c>
       <c r="K234" s="1">
-        <v>225</v>
+        <v>691</v>
       </c>
     </row>
     <row r="235" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9367,22 +9364,22 @@
         <v>10</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E235" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F235" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G235" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H235" s="1">
-        <v>184639.44</v>
+        <v>8595.7000000000007</v>
       </c>
       <c r="I235" s="1" t="s">
         <v>67</v>
@@ -9391,7 +9388,7 @@
         <v>68</v>
       </c>
       <c r="K235" s="1">
-        <v>691</v>
+        <v>49</v>
       </c>
     </row>
     <row r="236" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9402,7 +9399,7 @@
         <v>10</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D236" s="3" t="s">
         <v>14</v>
@@ -9411,13 +9408,13 @@
         <v>11</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G236" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H236" s="1">
-        <v>8595.7000000000007</v>
+        <v>67263.41</v>
       </c>
       <c r="I236" s="1" t="s">
         <v>67</v>
@@ -9426,7 +9423,7 @@
         <v>68</v>
       </c>
       <c r="K236" s="1">
-        <v>49</v>
+        <v>346</v>
       </c>
     </row>
     <row r="237" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9437,22 +9434,22 @@
         <v>10</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D237" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E237" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F237" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G237" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H237" s="1">
-        <v>67263.41</v>
+        <v>9549.2000000000007</v>
       </c>
       <c r="I237" s="1" t="s">
         <v>67</v>
@@ -9461,7 +9458,7 @@
         <v>68</v>
       </c>
       <c r="K237" s="1">
-        <v>346</v>
+        <v>102</v>
       </c>
     </row>
     <row r="238" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9472,7 +9469,7 @@
         <v>10</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D238" s="3" t="s">
         <v>14</v>
@@ -9481,13 +9478,13 @@
         <v>12</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H238" s="1">
-        <v>9549.2000000000007</v>
+        <v>67032.55</v>
       </c>
       <c r="I238" s="1" t="s">
         <v>67</v>
@@ -9496,7 +9493,7 @@
         <v>68</v>
       </c>
       <c r="K238" s="1">
-        <v>102</v>
+        <v>232</v>
       </c>
     </row>
     <row r="239" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9507,31 +9504,31 @@
         <v>10</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D239" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E239" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F239" s="1" t="s">
-        <v>268</v>
+        <v>15</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>269</v>
+        <v>16</v>
       </c>
       <c r="H239" s="1">
-        <v>67032.55</v>
+        <v>17039.36</v>
       </c>
       <c r="I239" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="J239" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="K239" s="1">
-        <v>232</v>
+        <v>127</v>
       </c>
     </row>
     <row r="240" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -9542,13 +9539,13 @@
         <v>10</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D240" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E240" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>15</v>
@@ -9557,7 +9554,7 @@
         <v>16</v>
       </c>
       <c r="H240" s="1">
-        <v>17039.36</v>
+        <v>21155.03</v>
       </c>
       <c r="I240" s="1" t="s">
         <v>17</v>
@@ -9566,41 +9563,6 @@
         <v>81</v>
       </c>
       <c r="K240" s="1">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="241" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B241" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D241" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E241" s="1">
-        <v>14</v>
-      </c>
-      <c r="F241" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G241" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H241" s="1">
-        <v>21155.03</v>
-      </c>
-      <c r="I241" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J241" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K241" s="1">
         <v>147</v>
       </c>
     </row>

</xml_diff>